<commit_message>
check mistakes in 'checkData'
</commit_message>
<xml_diff>
--- a/WaterData.xlsx
+++ b/WaterData.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr showObjects="all"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Water data" sheetId="1" r:id="rId2" state="visible"/>
+    <sheet name="Water data" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" iterateDelta="0.0001" refMode="A1"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="10">
   <si>
     <t xml:space="preserve">Дата</t>
   </si>
@@ -37,19 +37,25 @@
     <t xml:space="preserve">ГВС</t>
   </si>
   <si>
-    <t>345</t>
-  </si>
-  <si>
     <t xml:space="preserve">  (11.20.2022)</t>
   </si>
   <si>
-    <t>34</t>
+    <t xml:space="preserve">34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20.11.2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
@@ -87,14 +93,14 @@
     </fill>
   </fills>
   <borders count="2">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
       <right/>
       <top/>
@@ -104,8 +110,8 @@
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom"/>
-      <protection hidden="false" locked="true"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
@@ -129,16 +135,16 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom"/>
-      <protection hidden="false" locked="true"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom"/>
-      <protection hidden="false" locked="true"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -154,71 +160,122 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr>
-    <pageSetUpPr/>
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView showGridLines="true" showRowColHeaders="true" showZeros="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection activeCell="B3" activeCellId="0" pane="topLeft" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="true" max="1" min="1" width="15.8"/>
-    <col customWidth="true" max="2" min="2" width="14.46"/>
-    <col customWidth="true" max="3" min="3" width="8.7"/>
-    <col customWidth="true" max="4" min="4" width="11.34"/>
-    <col customWidth="true" max="5" min="5" style="1" width="11.34"/>
-    <col customWidth="true" max="8" min="8" width="10.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.68"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.8">
-      <c r="A1" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" ht="13.8">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <printOptions gridLinesSet="true"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup cellComments="none" copies="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" verticalDpi="300"/>
-  <headerFooter/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
next work with cold_data
</commit_message>
<xml_diff>
--- a/WaterData.xlsx
+++ b/WaterData.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr showObjects="all"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Water data" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Water data" sheetId="1" r:id="rId2" state="visible"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr iterateCount="100" iterateDelta="0.0001" refMode="A1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t xml:space="preserve">Дата</t>
   </si>
@@ -50,12 +50,15 @@
   </si>
   <si>
     <t xml:space="preserve">123</t>
+  </si>
+  <si>
+    <t>21.11.2022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
@@ -93,14 +96,14 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin"/>
       <right/>
       <top/>
@@ -110,8 +113,8 @@
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <alignment horizontal="general" vertical="bottom"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
@@ -135,16 +138,16 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <alignment horizontal="general" vertical="bottom"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <alignment horizontal="general" vertical="bottom"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+      <alignment horizontal="general" vertical="bottom"/>
+      <protection hidden="false" locked="true"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -160,122 +163,125 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
+  <sheetPr>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView showGridLines="true" showRowColHeaders="true" showZeros="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection activeCell="B9" activeCellId="0" pane="topLeft" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.68"/>
+    <col customWidth="true" max="1" min="1" width="15.8"/>
+    <col customWidth="true" max="2" min="2" width="14.46"/>
+    <col customWidth="true" max="3" min="3" width="8.7"/>
+    <col customWidth="true" max="4" min="4" width="11.34"/>
+    <col customWidth="true" max="5" min="5" style="1" width="11.34"/>
+    <col customWidth="true" max="8" min="8" width="10.68"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" ht="13.8">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" ht="13.8">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" ht="13.8">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="0" t="s">
+    <row r="4" ht="13.8">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="0" t="n">
+    <row r="5" ht="13.8">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="n">
         <v>123</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="0" t="n">
+    <row r="6" ht="13.8">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="n">
         <v>45</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="0" t="n">
+    <row r="7" ht="13.8">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="n">
         <v>12</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="0" t="n">
+    <row r="8" ht="13.8">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="0" t="n">
+    <row r="9" ht="13.8">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
         <v>2</v>
       </c>
+      <c r="E9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9">
+        <v>123.00</v>
+      </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <printOptions gridLinesSet="true"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup cellComments="none" copies="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>